<commit_message>
make import excel for kepesertaan
</commit_message>
<xml_diff>
--- a/public/files/2.xlsx
+++ b/public/files/2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bagus\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B8661C-5598-490C-9014-6CC9A0EAB211}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA6F54B4-5586-4741-A089-D2B334B9665C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{542E7A8D-D870-47CC-9729-60FBA3D964EF}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>018211</t>
   </si>
@@ -45,13 +45,61 @@
   </si>
   <si>
     <t>K/1</t>
+  </si>
+  <si>
+    <t>PAHUPL-PUSAT800-201812, PAHUPL, 01-12-2018, ISMAIL, 17-12-2018 11:51:56</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>NO Peserta</t>
+  </si>
+  <si>
+    <t>NIP</t>
+  </si>
+  <si>
+    <t>Nama Peserta</t>
+  </si>
+  <si>
+    <t>Unit kerja</t>
+  </si>
+  <si>
+    <t>Golongan</t>
+  </si>
+  <si>
+    <t>Stt</t>
+  </si>
+  <si>
+    <t>Gaji pokok</t>
+  </si>
+  <si>
+    <t>Gaji Pns</t>
+  </si>
+  <si>
+    <t>PHDP</t>
+  </si>
+  <si>
+    <t>Saat ini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mutasi </t>
+  </si>
+  <si>
+    <t>Kawin</t>
+  </si>
+  <si>
+    <t>Dari</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+  </numFmts>
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,6 +121,19 @@
       <sz val="10"/>
       <name val="Arial "/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -82,7 +143,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -90,11 +151,68 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -114,9 +232,54 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
+    <cellStyle name="Comma [0] 2 2" xfId="3" xr:uid="{D0104E6A-DE7F-44EA-B5FF-53F8564950DA}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 17 2" xfId="1" xr:uid="{E5791811-940A-4309-A4D3-AF398CFB551D}"/>
+    <cellStyle name="Normal 2 10" xfId="4" xr:uid="{04CFDFDE-C6C5-4580-9537-C75C52186AD9}"/>
+    <cellStyle name="Normal 2 2" xfId="2" xr:uid="{BA16BB97-3CBB-4BAD-B307-20FF69DD1B04}"/>
+    <cellStyle name="Normal 3" xfId="5" xr:uid="{C582C00F-65DA-4133-94C5-EC8DA3BC1B90}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -428,49 +591,209 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66736C23-AF2B-4A79-B8C8-8ED7E2B15B4D}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="K7" sqref="K7:K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1"/>
-      <c r="B1" s="1">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="B7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="13"/>
+      <c r="H7" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="B8" s="11"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="18"/>
+      <c r="I8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="21"/>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="B9" s="11"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="19"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="22"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="B10" s="1">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4">
+      <c r="F10" s="4">
         <v>101</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="4" t="s">
+      <c r="G10" s="5"/>
+      <c r="H10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="7">
+      <c r="J10" s="7">
         <v>1552800</v>
       </c>
-      <c r="K1" s="7">
+      <c r="K10" s="7">
         <v>0</v>
       </c>
-      <c r="L1" s="8">
+      <c r="L10" s="8">
         <v>1552800</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="J7:J9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="L7:L9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:H9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>